<commit_message>
from Apex Apr21 2018
</commit_message>
<xml_diff>
--- a/R/Data/analyst_event_exceptions.xlsx
+++ b/R/Data/analyst_event_exceptions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\YChen\Documents\git\working_dir\R\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{1C6EEF22-3D51-48A7-B677-8FA059C1B848}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{BE53177C-3F90-4A26-B61A-14D5AE202317}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17175" windowHeight="9015" xr2:uid="{C578D2FB-8E40-47D6-9AC8-E8931500E00C}"/>
   </bookViews>
@@ -24,8 +24,42 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>YChen</author>
+  </authors>
+  <commentList>
+    <comment ref="F21" authorId="0" shapeId="0" xr:uid="{E4A47921-7A09-45E2-A5E6-EB747DF39129}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>YChen:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+mistake on Bloomberg Alert</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="24">
   <si>
     <t>B/D</t>
   </si>
@@ -61,6 +95,42 @@
   </si>
   <si>
     <t>seems like CICC only downgraded A share of New China Life, not the H share</t>
+  </si>
+  <si>
+    <t>04/19/2018</t>
+  </si>
+  <si>
+    <t>06:16:02</t>
+  </si>
+  <si>
+    <t>1033 HK Equity</t>
+  </si>
+  <si>
+    <t>1033 HK</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Target Px decreased to 2.913 by J.P. Morgan</t>
+  </si>
+  <si>
+    <t>RECOM_SMALL</t>
+  </si>
+  <si>
+    <t>06:14:02</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Target Px decreased to .94 by J.P. Morgan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TP+ </t>
+  </si>
+  <si>
+    <t>J.P. Morgan</t>
+  </si>
+  <si>
+    <t>SINOPEC OILFIE-H</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TP- </t>
   </si>
 </sst>
 </file>
@@ -70,13 +140,26 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.00_);[Red]\(0.00\)"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -124,8 +207,8 @@
 <volTypes xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <volType type="realTimeData">
     <main first="bloomberg.rtd">
-      <tp>
-        <v>43118</v>
+      <tp t="e">
+        <v>#N/A</v>
         <stp/>
         <stp>##V3_BDHV12</stp>
         <stp>3800 hk equity</stp>
@@ -439,17 +522,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A19FC911-8CEE-40E9-B9FF-10E4FB1F580B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A19FC911-8CEE-40E9-B9FF-10E4FB1F580B}">
   <dimension ref="A2:R44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
@@ -688,19 +772,141 @@
       <c r="B20" s="1"/>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B21" s="1"/>
+      <c r="A21" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" t="s">
+        <v>14</v>
+      </c>
+      <c r="D21" t="s">
+        <v>15</v>
+      </c>
+      <c r="E21" t="s">
+        <v>16</v>
+      </c>
+      <c r="G21" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B22" s="1"/>
+      <c r="A22" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22" t="s">
+        <v>18</v>
+      </c>
+      <c r="C22" t="s">
+        <v>14</v>
+      </c>
+      <c r="D22" t="s">
+        <v>15</v>
+      </c>
+      <c r="E22" t="s">
+        <v>19</v>
+      </c>
+      <c r="G22" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B23" s="1"/>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B24" s="1"/>
+      <c r="A24">
+        <v>60</v>
+      </c>
+      <c r="B24" t="s">
+        <v>0</v>
+      </c>
+      <c r="C24" t="s">
+        <v>20</v>
+      </c>
+      <c r="D24" s="1">
+        <v>43209</v>
+      </c>
+      <c r="E24" t="s">
+        <v>21</v>
+      </c>
+      <c r="F24" t="s">
+        <v>22</v>
+      </c>
+      <c r="H24">
+        <v>157.78761061946901</v>
+      </c>
+      <c r="I24">
+        <v>-9.7345132743362797</v>
+      </c>
+      <c r="J24" s="2">
+        <v>185.58823529411799</v>
+      </c>
+      <c r="K24">
+        <v>131.55802563264999</v>
+      </c>
+      <c r="L24">
+        <v>4.1868916</v>
+      </c>
+      <c r="M24">
+        <v>3.0678559999999999</v>
+      </c>
+      <c r="O24">
+        <v>1</v>
+      </c>
+      <c r="P24">
+        <v>1</v>
+      </c>
+      <c r="R24">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B25" s="1"/>
+      <c r="A25">
+        <v>61</v>
+      </c>
+      <c r="B25" t="s">
+        <v>0</v>
+      </c>
+      <c r="C25" t="s">
+        <v>23</v>
+      </c>
+      <c r="D25" s="1">
+        <v>43209</v>
+      </c>
+      <c r="E25" t="s">
+        <v>21</v>
+      </c>
+      <c r="F25" t="s">
+        <v>22</v>
+      </c>
+      <c r="H25">
+        <v>-16.814159292035399</v>
+      </c>
+      <c r="I25">
+        <v>-9.7345132743362797</v>
+      </c>
+      <c r="J25" s="2">
+        <v>-7.8431372549019702</v>
+      </c>
+      <c r="K25">
+        <v>-25.278220358842699</v>
+      </c>
+      <c r="L25">
+        <v>4.1868916</v>
+      </c>
+      <c r="M25">
+        <v>3.0678559999999999</v>
+      </c>
+      <c r="O25">
+        <v>1</v>
+      </c>
+      <c r="P25">
+        <v>1</v>
+      </c>
+      <c r="R25">
+        <v>-0.5</v>
+      </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
@@ -761,5 +967,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>